<commit_message>
added DFT based steric fingerprint for SM7 and SM8
</commit_message>
<xml_diff>
--- a/obelix_ml_pipeline/data/substrate_representations/raw_data_processing/substrate_dft_steric_fingerprint/substrate_atom_mapping.xlsx
+++ b/obelix_ml_pipeline/data/substrate_representations/raw_data_processing/substrate_dft_steric_fingerprint/substrate_atom_mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Substrate</t>
   </si>
@@ -73,6 +73,24 @@
   </si>
   <si>
     <t>OC(/C(NC(C)=O)=C/C1=CC=CC=C1)=O</t>
+  </si>
+  <si>
+    <t>SM7</t>
+  </si>
+  <si>
+    <t>SM8</t>
+  </si>
+  <si>
+    <t>C/C(C(O)=O)=C\C1=CC=CC=C1</t>
+  </si>
+  <si>
+    <t>C=C(C(O)=O)C1=CC=CC=C1</t>
+  </si>
+  <si>
+    <t>SM7_only_after_DFT.xyz</t>
+  </si>
+  <si>
+    <t>SM8_only_after_DFT.xyz</t>
   </si>
 </sst>
 </file>
@@ -132,19 +150,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>483578</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>89297</xdr:rowOff>
+      <xdr:colOff>235323</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>351692</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>116350</xdr:rowOff>
+      <xdr:colOff>159167</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>42378</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -163,8 +181,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="483578" y="1613297"/>
-          <a:ext cx="3516922" cy="2313053"/>
+          <a:off x="235323" y="1367117"/>
+          <a:ext cx="3554550" cy="5533261"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -439,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +581,64 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>